<commit_message>
Updating test data to include saint martin as edgecase
</commit_message>
<xml_diff>
--- a/tests/testthat/20220712-mpx-test-data.xlsx
+++ b/tests/testthat/20220712-mpx-test-data.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oet5\mpox\savimpx\tests\testthat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7AF8AB25-69C3-4038-9E77-AB58A5B82C4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{875050D7-2FA8-4C28-AA29-DCA585709BA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1040" yWindow="1040" windowWidth="28800" windowHeight="15500"/>
+    <workbookView xWindow="1040" yWindow="1040" windowWidth="28800" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="20220712-mpx-test-data" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
   <si>
     <t>Country</t>
   </si>
@@ -212,12 +212,15 @@
   </si>
   <si>
     <t>Venezuela</t>
+  </si>
+  <si>
+    <t>Saint Martin</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1052,11 +1055,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B64"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="F62" sqref="F62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1573,7 +1576,16 @@
         <v>1</v>
       </c>
     </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>64</v>
+      </c>
+      <c r="B65">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>